<commit_message>
Adicionando Código (Samuel - 15/07)
</commit_message>
<xml_diff>
--- a/Main/Main/modelo.xlsx
+++ b/Main/Main/modelo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i.peres\Pictures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos Internos\Braspor\Main\Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535516F0-082E-4098-9ED2-3A5B70BE56A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B70EAD7-A6A2-46FD-94CE-67D8C68EE504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6759B5E2-5784-4CCD-A2A3-043F6CC4644C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6759B5E2-5784-4CCD-A2A3-043F6CC4644C}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Relatório de processo</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Operador</t>
-  </si>
-  <si>
-    <t>Matéria Prima</t>
   </si>
   <si>
     <t>Matéria Prima:</t>
@@ -49,9 +46,6 @@
   </si>
   <si>
     <t>Nome Operador</t>
-  </si>
-  <si>
-    <t>Descrição Produto</t>
   </si>
   <si>
     <t>Tempo execução</t>
@@ -70,6 +64,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Observação do Processo</t>
   </si>
 </sst>
 </file>
@@ -298,7 +295,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -577,7 +574,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>219587</xdr:colOff>
+      <xdr:colOff>219588</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>431652</xdr:rowOff>
     </xdr:to>
@@ -921,19 +918,19 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
     <col min="9" max="19" width="9.140625" style="12"/>
   </cols>
   <sheetData>
@@ -953,7 +950,7 @@
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -973,7 +970,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="21">
         <v>45209</v>
@@ -984,10 +981,10 @@
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="19"/>
@@ -1026,29 +1023,27 @@
     </row>
     <row r="8" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="H8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1069,6 +1064,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c71f299d-61df-4ef7-abf1-9fbd4ad59504">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="50c9d8df-c338-426b-b4a4-fac303072325" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FEA0655D54C1D543A33824F64EBEACB7" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="757f678880176b38ef5c27711a5e0e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c71f299d-61df-4ef7-abf1-9fbd4ad59504" xmlns:ns3="27ad76c2-a786-4371-9940-3823bf9cf127" xmlns:ns4="50c9d8df-c338-426b-b4a4-fac303072325" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9454706c19a4b1745b9733898b7dd59" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="c71f299d-61df-4ef7-abf1-9fbd4ad59504"/>
@@ -1316,42 +1331,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c71f299d-61df-4ef7-abf1-9fbd4ad59504">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="50c9d8df-c338-426b-b4a4-fac303072325" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ABF1BC5-2436-416B-9A76-5CEC114F4DC2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{073E3BFD-1386-435F-90F1-944A1DEA0091}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c71f299d-61df-4ef7-abf1-9fbd4ad59504"/>
-    <ds:schemaRef ds:uri="27ad76c2-a786-4371-9940-3823bf9cf127"/>
-    <ds:schemaRef ds:uri="50c9d8df-c338-426b-b4a4-fac303072325"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1375,9 +1358,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{073E3BFD-1386-435F-90F1-944A1DEA0091}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ABF1BC5-2436-416B-9A76-5CEC114F4DC2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c71f299d-61df-4ef7-abf1-9fbd4ad59504"/>
+    <ds:schemaRef ds:uri="27ad76c2-a786-4371-9940-3823bf9cf127"/>
+    <ds:schemaRef ds:uri="50c9d8df-c338-426b-b4a4-fac303072325"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>